<commit_message>
update readme for running paper analyses
</commit_message>
<xml_diff>
--- a/paper/data/DataSets.xlsx
+++ b/paper/data/DataSets.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Error Rate</t>
   </si>
@@ -48,16 +48,13 @@
     <t>GM12878 WGBS</t>
   </si>
   <si>
-    <t>Unknown</t>
-  </si>
-  <si>
-    <t>16,999*</t>
-  </si>
-  <si>
-    <t>1,020,017*</t>
-  </si>
-  <si>
     <t>Reads w/ Adapters</t>
+  </si>
+  <si>
+    <t>K562 mRNA-seq</t>
+  </si>
+  <si>
+    <t>For real data sets, error rates are estimated from base qualities and adapter content is identified as exact matches to the first 35 bp of adapter sequence.</t>
   </si>
 </sst>
 </file>
@@ -132,7 +129,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
@@ -150,6 +147,9 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
@@ -496,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -525,7 +525,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>4</v>
@@ -595,8 +595,8 @@
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>9</v>
+      <c r="B5" s="10">
+        <v>2.7900000000000001E-2</v>
       </c>
       <c r="C5" s="5">
         <v>125</v>
@@ -604,10 +604,35 @@
       <c r="D5" s="4">
         <v>1000000</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="9">
+        <v>57130</v>
+      </c>
+      <c r="F5" s="9">
+        <v>3082003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="B6" s="10">
+        <v>4.3099999999999999E-2</v>
+      </c>
+      <c r="C6" s="5">
+        <v>75</v>
+      </c>
+      <c r="D6" s="4">
+        <v>6100265</v>
+      </c>
+      <c r="E6" s="3">
+        <v>14384</v>
+      </c>
+      <c r="F6" s="4">
+        <v>749451</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>